<commit_message>
Working on loanable funds model.
</commit_message>
<xml_diff>
--- a/LoanableFunds.xlsx
+++ b/LoanableFunds.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="840" windowWidth="42640" windowHeight="22700" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="1960" windowWidth="42640" windowHeight="22700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,6 +194,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -203,13 +210,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -562,11 +562,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2107430976"/>
-        <c:axId val="-2107258288"/>
+        <c:axId val="-2104253344"/>
+        <c:axId val="-2104249824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2107430976"/>
+        <c:axId val="-2104253344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,12 +623,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107258288"/>
+        <c:crossAx val="-2104249824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2107258288"/>
+        <c:axId val="-2104249824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107430976"/>
+        <c:crossAx val="-2104253344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1623,7 +1623,7 @@
   <dimension ref="B1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="229" zoomScaleNormal="229" zoomScalePageLayoutView="229" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B20"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,12 +1634,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="20" x14ac:dyDescent="0.25">
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E3" s="1" t="s">
@@ -1648,7 +1648,7 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I3">
@@ -1681,19 +1681,19 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <f>F5</f>
         <v>0</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <f t="shared" ref="C8:C18" si="0">(B8-$F$4)*$I$3*$E$4</f>
         <v>120</v>
       </c>
@@ -1703,11 +1703,11 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <f>B8+0.01</f>
         <v>0.01</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
@@ -1717,11 +1717,11 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <f t="shared" ref="B10:B20" si="1">B9+0.01</f>
         <v>0.02</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <f t="shared" si="0"/>
         <v>99.999999999999986</v>
       </c>
@@ -1731,11 +1731,11 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -1745,11 +1745,11 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>79.999999999999986</v>
       </c>
@@ -1759,11 +1759,11 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
         <v>69.999999999999986</v>
       </c>
@@ -1773,11 +1773,11 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <f t="shared" si="1"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <f t="shared" si="0"/>
         <v>59.999999999999993</v>
       </c>
@@ -1787,11 +1787,11 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <f t="shared" si="0"/>
         <v>49.999999999999986</v>
       </c>
@@ -1799,26 +1799,26 @@
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="11"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="8"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <f t="shared" si="0"/>
         <v>39.999999999999993</v>
       </c>
@@ -1841,11 +1841,11 @@
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1867,11 +1867,11 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <f t="shared" si="1"/>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <f t="shared" si="0"/>
         <v>20.000000000000004</v>
       </c>
@@ -1881,11 +1881,11 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <f t="shared" si="1"/>
         <v>0.10999999999999999</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <f>(B19-$F$4)*$I$3*$E$4</f>
         <v>10.000000000000009</v>
       </c>
@@ -1895,11 +1895,11 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <f t="shared" si="1"/>
         <v>0.11999999999999998</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <f>(B20-$F$4)*$I$3*$E$4</f>
         <v>1.3877787807814457E-14</v>
       </c>

</xml_diff>